<commit_message>
update readme, docs and some fix
</commit_message>
<xml_diff>
--- a/dati_test.xlsx
+++ b/dati_test.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Foglio1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Foglio1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -739,7 +739,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Verificare l'accesso con credenziali valide</t>
+          <t>Verifica utenza non loggata</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">

</xml_diff>

<commit_message>
add app-use in requirements
</commit_message>
<xml_diff>
--- a/dati_test.xlsx
+++ b/dati_test.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Foglio1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Foglio1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -620,7 +620,7 @@
         </is>
       </c>
       <c r="D4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -748,7 +748,7 @@
         </is>
       </c>
       <c r="D7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
fix cell visualization for long text
</commit_message>
<xml_diff>
--- a/dati_test.xlsx
+++ b/dati_test.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Foglio1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Foglio1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -748,7 +748,7 @@
         </is>
       </c>
       <c r="D7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -803,6 +803,38 @@
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr"/>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>TEST_CASE_8</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Verifica upload</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Apri il sito https://www.zamzar.com/ e clicca sull'icona "triangolo rovesciato" di fianco a"Choose file" e seleziona da URL, incolla https://avatars.githubusercontent.com/u/192012301?s=48&amp;v=4 e verifica l'upload</t>
+        </is>
+      </c>
+      <c r="D9" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>web</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>